<commit_message>
v2. fix spelling in excel_test.xlsx
</commit_message>
<xml_diff>
--- a/excel_test.xlsx
+++ b/excel_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ah Hyun Kim\Documents\tortoisegit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5775D264-DDB4-4E96-84C3-6739AC3B7F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7940DC6C-E002-4DAE-AC5A-864BBBE9E0AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,11 +27,11 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>id tset</t>
+    <t>test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
+    <t>id test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -360,19 +360,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>